<commit_message>
ran the daily check. updating files.
</commit_message>
<xml_diff>
--- a/data/tbl_churn_data/xlsx/2016_Churn.xlsx
+++ b/data/tbl_churn_data/xlsx/2016_Churn.xlsx
@@ -1,27 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\cdss\admd\Central Office\RSB\DSS\Employee Folders\MeganVisel\CalFresh Churn Report\2016\Data\Churn\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="26835" windowHeight="13350" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="26835" windowHeight="13350" tabRatio="711" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CY2016 Q1 Churn Statewide Summa" sheetId="2" r:id="rId1"/>
     <sheet name="CY2016 Q2 Churn Statewide Summa" sheetId="3" r:id="rId2"/>
     <sheet name="CY2016 Q3 Churn Statewide Summa" sheetId="4" r:id="rId3"/>
+    <sheet name="CY2016 Q4 Churn Statewide Summa" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="IDX" localSheetId="0">'CY2016 Q1 Churn Statewide Summa'!$A$1</definedName>
     <definedName name="IDX" localSheetId="1">'CY2016 Q2 Churn Statewide Summa'!$A$1</definedName>
     <definedName name="IDX" localSheetId="2">'CY2016 Q3 Churn Statewide Summa'!$A$1</definedName>
+    <definedName name="IDX" localSheetId="3">'CY2016 Q4 Churn Statewide Summa'!$A$1</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="123">
   <si>
     <t>Federal Data Reporting and Analysis Bureau</t>
   </si>
@@ -385,11 +392,17 @@
   <si>
     <t>CY2016 Q3 (July - September) Churn Statewide Summary Report</t>
   </si>
+  <si>
+    <t>Report Run on 05MAY2017</t>
+  </si>
+  <si>
+    <t>CY2016 Q4 (October - December) Churn Statewide Summary Report</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="23">
     <font>
       <sz val="11"/>
@@ -954,7 +967,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1002,6 +1015,15 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1074,6 +1096,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1121,7 +1146,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1154,9 +1179,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1189,6 +1231,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1406,7 +1465,7 @@
       <c r="A4" s="3"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4">
@@ -1468,7 +1527,7 @@
       </c>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="19"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1528,7 +1587,7 @@
       </c>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="19"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1588,7 +1647,7 @@
       </c>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="19"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
@@ -1648,7 +1707,7 @@
       </c>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="19"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
@@ -1702,7 +1761,7 @@
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="19"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5">
@@ -1754,7 +1813,7 @@
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="19"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
@@ -1800,7 +1859,7 @@
       <c r="T11" s="5"/>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="19"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1838,7 +1897,7 @@
       <c r="T12" s="5"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="19"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1874,7 +1933,7 @@
       <c r="T13" s="5"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="19"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1908,7 +1967,7 @@
       <c r="T14" s="5"/>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="19"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1936,7 +1995,7 @@
       <c r="T15" s="5"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="20"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -5636,7 +5695,7 @@
   <dimension ref="A1:T75"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5654,7 +5713,8 @@
     <col min="16" max="16" width="12.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="10.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="11"/>
+    <col min="21" max="21" width="9" style="11" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -5676,7 +5736,7 @@
       <c r="A4" s="16"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="24" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="15">
@@ -5738,7 +5798,7 @@
       </c>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="22"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="14" t="s">
         <v>4</v>
       </c>
@@ -5798,7 +5858,7 @@
       </c>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="22"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="14" t="s">
         <v>5</v>
       </c>
@@ -5858,7 +5918,7 @@
       </c>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="22"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="14" t="s">
         <v>6</v>
       </c>
@@ -5918,7 +5978,7 @@
       </c>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="22"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="14" t="s">
         <v>7</v>
       </c>
@@ -5972,7 +6032,7 @@
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="22"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14">
@@ -6024,7 +6084,7 @@
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="22"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14" t="s">
@@ -6070,7 +6130,7 @@
       <c r="T11" s="14"/>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="22"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -6108,7 +6168,7 @@
       <c r="T12" s="14"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="22"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -6144,7 +6204,7 @@
       <c r="T13" s="14"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="22"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
@@ -6178,7 +6238,7 @@
       <c r="T14" s="14"/>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="22"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -6206,7 +6266,7 @@
       <c r="T15" s="14"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="23"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
@@ -9904,7 +9964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T75"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -9943,7 +10003,7 @@
       <c r="A4" s="3"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="8">
@@ -10005,7 +10065,7 @@
       </c>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="19"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
@@ -10065,7 +10125,7 @@
       </c>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="19"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="9" t="s">
         <v>5</v>
       </c>
@@ -10125,7 +10185,7 @@
       </c>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="19"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
@@ -10185,7 +10245,7 @@
       </c>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="19"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
@@ -10239,7 +10299,7 @@
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="19"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9">
@@ -10291,7 +10351,7 @@
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="19"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9" t="s">
@@ -10337,7 +10397,7 @@
       <c r="T11" s="9"/>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="19"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -10375,7 +10435,7 @@
       <c r="T12" s="9"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="19"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -10411,7 +10471,7 @@
       <c r="T13" s="9"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="19"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -10445,7 +10505,7 @@
       <c r="T14" s="9"/>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="19"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -10473,7 +10533,7 @@
       <c r="T15" s="9"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="20"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -14164,4 +14224,4272 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T75"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="7.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="25.5">
+      <c r="A2" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="3"/>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="18">
+        <v>1</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="18">
+        <v>2</v>
+      </c>
+      <c r="I5" s="18">
+        <v>3</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="18">
+        <v>4</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="P5" s="18">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="R5" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="S5" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="T5" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="22"/>
+      <c r="B6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="S6" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="T6" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="22"/>
+      <c r="B7" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="R7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="S7" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="T7" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="22"/>
+      <c r="B8" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="P8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="R8" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="S8" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="T8" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="22"/>
+      <c r="B9" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="P9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="22"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19">
+        <v>30</v>
+      </c>
+      <c r="E10" s="19">
+        <v>60</v>
+      </c>
+      <c r="F10" s="19">
+        <v>90</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="O10" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="P10" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="22"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="P11" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="22"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="M12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="O12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="P12" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="22"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19">
+        <v>90</v>
+      </c>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="O13" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="P13" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="22"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="P14" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="22"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19">
+        <v>30</v>
+      </c>
+      <c r="N15" s="19">
+        <v>60</v>
+      </c>
+      <c r="O15" s="19">
+        <v>90</v>
+      </c>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="23"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="N16" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="O16" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="7">
+        <v>443375</v>
+      </c>
+      <c r="C17" s="7">
+        <v>199703</v>
+      </c>
+      <c r="D17" s="7">
+        <v>67611</v>
+      </c>
+      <c r="E17" s="7">
+        <v>28394</v>
+      </c>
+      <c r="F17" s="7">
+        <v>17543</v>
+      </c>
+      <c r="G17" s="7">
+        <v>130124</v>
+      </c>
+      <c r="H17" s="7">
+        <v>11.8</v>
+      </c>
+      <c r="I17" s="7">
+        <v>530804</v>
+      </c>
+      <c r="J17" s="7">
+        <v>353874</v>
+      </c>
+      <c r="K17" s="7">
+        <v>176930</v>
+      </c>
+      <c r="L17" s="7">
+        <v>99182</v>
+      </c>
+      <c r="M17" s="7">
+        <v>81555</v>
+      </c>
+      <c r="N17" s="7">
+        <v>11025</v>
+      </c>
+      <c r="O17" s="7">
+        <v>6602</v>
+      </c>
+      <c r="P17" s="7">
+        <v>29.4</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>25.61</v>
+      </c>
+      <c r="R17" s="7">
+        <v>15.25</v>
+      </c>
+      <c r="S17" s="7">
+        <v>22.37</v>
+      </c>
+      <c r="T17" s="7">
+        <v>18.39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="7">
+        <v>13059</v>
+      </c>
+      <c r="C18" s="7">
+        <v>5899</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1491</v>
+      </c>
+      <c r="E18" s="7">
+        <v>851</v>
+      </c>
+      <c r="F18" s="7">
+        <v>541</v>
+      </c>
+      <c r="G18" s="7">
+        <v>4277</v>
+      </c>
+      <c r="H18" s="7">
+        <v>6</v>
+      </c>
+      <c r="I18" s="7">
+        <v>13505</v>
+      </c>
+      <c r="J18" s="7">
+        <v>9812</v>
+      </c>
+      <c r="K18" s="7">
+        <v>3693</v>
+      </c>
+      <c r="L18" s="7">
+        <v>1923</v>
+      </c>
+      <c r="M18" s="7">
+        <v>1152</v>
+      </c>
+      <c r="N18" s="7">
+        <v>478</v>
+      </c>
+      <c r="O18" s="7">
+        <v>293</v>
+      </c>
+      <c r="P18" s="7">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>22.08</v>
+      </c>
+      <c r="R18" s="7">
+        <v>11.42</v>
+      </c>
+      <c r="S18" s="7">
+        <v>14.73</v>
+      </c>
+      <c r="T18" s="7">
+        <v>8.82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="7">
+        <v>16</v>
+      </c>
+      <c r="C19" s="7">
+        <v>9</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0</v>
+      </c>
+      <c r="G19" s="7">
+        <v>6</v>
+      </c>
+      <c r="H19" s="7">
+        <v>11.7</v>
+      </c>
+      <c r="I19" s="7">
+        <v>25</v>
+      </c>
+      <c r="J19" s="7">
+        <v>13</v>
+      </c>
+      <c r="K19" s="7">
+        <v>12</v>
+      </c>
+      <c r="L19" s="7">
+        <v>2</v>
+      </c>
+      <c r="M19" s="7">
+        <v>1</v>
+      </c>
+      <c r="N19" s="7">
+        <v>0</v>
+      </c>
+      <c r="O19" s="7">
+        <v>1</v>
+      </c>
+      <c r="P19" s="7">
+        <v>22.7</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>6.25</v>
+      </c>
+      <c r="R19" s="7">
+        <v>0</v>
+      </c>
+      <c r="S19" s="7">
+        <v>12.5</v>
+      </c>
+      <c r="T19" s="7">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="7">
+        <v>396</v>
+      </c>
+      <c r="C20" s="7">
+        <v>197</v>
+      </c>
+      <c r="D20" s="7">
+        <v>33</v>
+      </c>
+      <c r="E20" s="7">
+        <v>24</v>
+      </c>
+      <c r="F20" s="7">
+        <v>12</v>
+      </c>
+      <c r="G20" s="7">
+        <v>130</v>
+      </c>
+      <c r="H20" s="7">
+        <v>14</v>
+      </c>
+      <c r="I20" s="7">
+        <v>558</v>
+      </c>
+      <c r="J20" s="7">
+        <v>313</v>
+      </c>
+      <c r="K20" s="7">
+        <v>245</v>
+      </c>
+      <c r="L20" s="7">
+        <v>105</v>
+      </c>
+      <c r="M20" s="7">
+        <v>93</v>
+      </c>
+      <c r="N20" s="7">
+        <v>7</v>
+      </c>
+      <c r="O20" s="7">
+        <v>5</v>
+      </c>
+      <c r="P20" s="7">
+        <v>23.3</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>17.420000000000002</v>
+      </c>
+      <c r="R20" s="7">
+        <v>8.33</v>
+      </c>
+      <c r="S20" s="7">
+        <v>26.52</v>
+      </c>
+      <c r="T20" s="7">
+        <v>23.48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="7">
+        <v>4225</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1999</v>
+      </c>
+      <c r="D21" s="7">
+        <v>669</v>
+      </c>
+      <c r="E21" s="7">
+        <v>234</v>
+      </c>
+      <c r="F21" s="7">
+        <v>156</v>
+      </c>
+      <c r="G21" s="7">
+        <v>1167</v>
+      </c>
+      <c r="H21" s="7">
+        <v>17.7</v>
+      </c>
+      <c r="I21" s="7">
+        <v>4921</v>
+      </c>
+      <c r="J21" s="7">
+        <v>2819</v>
+      </c>
+      <c r="K21" s="7">
+        <v>2102</v>
+      </c>
+      <c r="L21" s="7">
+        <v>1197</v>
+      </c>
+      <c r="M21" s="7">
+        <v>1040</v>
+      </c>
+      <c r="N21" s="7">
+        <v>112</v>
+      </c>
+      <c r="O21" s="7">
+        <v>45</v>
+      </c>
+      <c r="P21" s="7">
+        <v>27</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>25.07</v>
+      </c>
+      <c r="R21" s="7">
+        <v>15.83</v>
+      </c>
+      <c r="S21" s="7">
+        <v>28.33</v>
+      </c>
+      <c r="T21" s="7">
+        <v>24.62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="7">
+        <v>584</v>
+      </c>
+      <c r="C22" s="7">
+        <v>307</v>
+      </c>
+      <c r="D22" s="7">
+        <v>52</v>
+      </c>
+      <c r="E22" s="7">
+        <v>28</v>
+      </c>
+      <c r="F22" s="7">
+        <v>23</v>
+      </c>
+      <c r="G22" s="7">
+        <v>174</v>
+      </c>
+      <c r="H22" s="7">
+        <v>11.7</v>
+      </c>
+      <c r="I22" s="7">
+        <v>873</v>
+      </c>
+      <c r="J22" s="7">
+        <v>508</v>
+      </c>
+      <c r="K22" s="7">
+        <v>365</v>
+      </c>
+      <c r="L22" s="7">
+        <v>240</v>
+      </c>
+      <c r="M22" s="7">
+        <v>219</v>
+      </c>
+      <c r="N22" s="7">
+        <v>10</v>
+      </c>
+      <c r="O22" s="7">
+        <v>11</v>
+      </c>
+      <c r="P22" s="7">
+        <v>26.7</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>17.64</v>
+      </c>
+      <c r="R22" s="7">
+        <v>8.9</v>
+      </c>
+      <c r="S22" s="7">
+        <v>41.1</v>
+      </c>
+      <c r="T22" s="7">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="7">
+        <v>214</v>
+      </c>
+      <c r="C23" s="7">
+        <v>101</v>
+      </c>
+      <c r="D23" s="7">
+        <v>24</v>
+      </c>
+      <c r="E23" s="7">
+        <v>4</v>
+      </c>
+      <c r="F23" s="7">
+        <v>8</v>
+      </c>
+      <c r="G23" s="7">
+        <v>77</v>
+      </c>
+      <c r="H23" s="7">
+        <v>22</v>
+      </c>
+      <c r="I23" s="7">
+        <v>215</v>
+      </c>
+      <c r="J23" s="7">
+        <v>111</v>
+      </c>
+      <c r="K23" s="7">
+        <v>104</v>
+      </c>
+      <c r="L23" s="7">
+        <v>68</v>
+      </c>
+      <c r="M23" s="7">
+        <v>63</v>
+      </c>
+      <c r="N23" s="7">
+        <v>1</v>
+      </c>
+      <c r="O23" s="7">
+        <v>4</v>
+      </c>
+      <c r="P23" s="7">
+        <v>25.7</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>16.82</v>
+      </c>
+      <c r="R23" s="7">
+        <v>11.21</v>
+      </c>
+      <c r="S23" s="7">
+        <v>31.78</v>
+      </c>
+      <c r="T23" s="7">
+        <v>29.44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="7">
+        <v>7925</v>
+      </c>
+      <c r="C24" s="7">
+        <v>4136</v>
+      </c>
+      <c r="D24" s="7">
+        <v>700</v>
+      </c>
+      <c r="E24" s="7">
+        <v>456</v>
+      </c>
+      <c r="F24" s="7">
+        <v>299</v>
+      </c>
+      <c r="G24" s="7">
+        <v>2334</v>
+      </c>
+      <c r="H24" s="7">
+        <v>12</v>
+      </c>
+      <c r="I24" s="7">
+        <v>7131</v>
+      </c>
+      <c r="J24" s="7">
+        <v>5434</v>
+      </c>
+      <c r="K24" s="7">
+        <v>1697</v>
+      </c>
+      <c r="L24" s="7">
+        <v>840</v>
+      </c>
+      <c r="M24" s="7">
+        <v>513</v>
+      </c>
+      <c r="N24" s="7">
+        <v>187</v>
+      </c>
+      <c r="O24" s="7">
+        <v>140</v>
+      </c>
+      <c r="P24" s="7">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>18.36</v>
+      </c>
+      <c r="R24" s="7">
+        <v>8.83</v>
+      </c>
+      <c r="S24" s="7">
+        <v>10.6</v>
+      </c>
+      <c r="T24" s="7">
+        <v>6.47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="7">
+        <v>566</v>
+      </c>
+      <c r="C25" s="7">
+        <v>248</v>
+      </c>
+      <c r="D25" s="7">
+        <v>123</v>
+      </c>
+      <c r="E25" s="7">
+        <v>27</v>
+      </c>
+      <c r="F25" s="7">
+        <v>18</v>
+      </c>
+      <c r="G25" s="7">
+        <v>150</v>
+      </c>
+      <c r="H25" s="7">
+        <v>10.7</v>
+      </c>
+      <c r="I25" s="7">
+        <v>812</v>
+      </c>
+      <c r="J25" s="7">
+        <v>511</v>
+      </c>
+      <c r="K25" s="7">
+        <v>301</v>
+      </c>
+      <c r="L25" s="7">
+        <v>261</v>
+      </c>
+      <c r="M25" s="7">
+        <v>247</v>
+      </c>
+      <c r="N25" s="7">
+        <v>9</v>
+      </c>
+      <c r="O25" s="7">
+        <v>5</v>
+      </c>
+      <c r="P25" s="7">
+        <v>27.7</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>29.68</v>
+      </c>
+      <c r="R25" s="7">
+        <v>21.73</v>
+      </c>
+      <c r="S25" s="7">
+        <v>46.11</v>
+      </c>
+      <c r="T25" s="7">
+        <v>43.64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="7">
+        <v>1771</v>
+      </c>
+      <c r="C26" s="7">
+        <v>829</v>
+      </c>
+      <c r="D26" s="7">
+        <v>277</v>
+      </c>
+      <c r="E26" s="7">
+        <v>87</v>
+      </c>
+      <c r="F26" s="7">
+        <v>74</v>
+      </c>
+      <c r="G26" s="7">
+        <v>504</v>
+      </c>
+      <c r="H26" s="7">
+        <v>10</v>
+      </c>
+      <c r="I26" s="7">
+        <v>2275</v>
+      </c>
+      <c r="J26" s="7">
+        <v>1223</v>
+      </c>
+      <c r="K26" s="7">
+        <v>1052</v>
+      </c>
+      <c r="L26" s="7">
+        <v>502</v>
+      </c>
+      <c r="M26" s="7">
+        <v>450</v>
+      </c>
+      <c r="N26" s="7">
+        <v>36</v>
+      </c>
+      <c r="O26" s="7">
+        <v>16</v>
+      </c>
+      <c r="P26" s="7">
+        <v>28</v>
+      </c>
+      <c r="Q26" s="7">
+        <v>24.73</v>
+      </c>
+      <c r="R26" s="7">
+        <v>15.64</v>
+      </c>
+      <c r="S26" s="7">
+        <v>28.35</v>
+      </c>
+      <c r="T26" s="7">
+        <v>25.41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="7">
+        <v>17976</v>
+      </c>
+      <c r="C27" s="7">
+        <v>5828</v>
+      </c>
+      <c r="D27" s="7">
+        <v>2959</v>
+      </c>
+      <c r="E27" s="7">
+        <v>1516</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1006</v>
+      </c>
+      <c r="G27" s="7">
+        <v>6667</v>
+      </c>
+      <c r="H27" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I27" s="7">
+        <v>25674</v>
+      </c>
+      <c r="J27" s="7">
+        <v>21605</v>
+      </c>
+      <c r="K27" s="7">
+        <v>4069</v>
+      </c>
+      <c r="L27" s="7">
+        <v>3311</v>
+      </c>
+      <c r="M27" s="7">
+        <v>2211</v>
+      </c>
+      <c r="N27" s="7">
+        <v>650</v>
+      </c>
+      <c r="O27" s="7">
+        <v>450</v>
+      </c>
+      <c r="P27" s="7">
+        <v>49</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>30.49</v>
+      </c>
+      <c r="R27" s="7">
+        <v>16.46</v>
+      </c>
+      <c r="S27" s="7">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="T27" s="7">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="7">
+        <v>373</v>
+      </c>
+      <c r="C28" s="7">
+        <v>175</v>
+      </c>
+      <c r="D28" s="7">
+        <v>46</v>
+      </c>
+      <c r="E28" s="7">
+        <v>27</v>
+      </c>
+      <c r="F28" s="7">
+        <v>20</v>
+      </c>
+      <c r="G28" s="7">
+        <v>105</v>
+      </c>
+      <c r="H28" s="7">
+        <v>12.3</v>
+      </c>
+      <c r="I28" s="7">
+        <v>499</v>
+      </c>
+      <c r="J28" s="7">
+        <v>278</v>
+      </c>
+      <c r="K28" s="7">
+        <v>221</v>
+      </c>
+      <c r="L28" s="7">
+        <v>93</v>
+      </c>
+      <c r="M28" s="7">
+        <v>80</v>
+      </c>
+      <c r="N28" s="7">
+        <v>6</v>
+      </c>
+      <c r="O28" s="7">
+        <v>7</v>
+      </c>
+      <c r="P28" s="7">
+        <v>23.3</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>24.93</v>
+      </c>
+      <c r="R28" s="7">
+        <v>12.33</v>
+      </c>
+      <c r="S28" s="7">
+        <v>24.93</v>
+      </c>
+      <c r="T28" s="7">
+        <v>21.45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="7">
+        <v>3325</v>
+      </c>
+      <c r="C29" s="7">
+        <v>1686</v>
+      </c>
+      <c r="D29" s="7">
+        <v>482</v>
+      </c>
+      <c r="E29" s="7">
+        <v>222</v>
+      </c>
+      <c r="F29" s="7">
+        <v>159</v>
+      </c>
+      <c r="G29" s="7">
+        <v>776</v>
+      </c>
+      <c r="H29" s="7">
+        <v>10.3</v>
+      </c>
+      <c r="I29" s="7">
+        <v>3525</v>
+      </c>
+      <c r="J29" s="7">
+        <v>1879</v>
+      </c>
+      <c r="K29" s="7">
+        <v>1646</v>
+      </c>
+      <c r="L29" s="7">
+        <v>1003</v>
+      </c>
+      <c r="M29" s="7">
+        <v>901</v>
+      </c>
+      <c r="N29" s="7">
+        <v>77</v>
+      </c>
+      <c r="O29" s="7">
+        <v>25</v>
+      </c>
+      <c r="P29" s="7">
+        <v>31.7</v>
+      </c>
+      <c r="Q29" s="7">
+        <v>25.95</v>
+      </c>
+      <c r="R29" s="7">
+        <v>14.5</v>
+      </c>
+      <c r="S29" s="7">
+        <v>30.17</v>
+      </c>
+      <c r="T29" s="7">
+        <v>27.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="7">
+        <v>3049</v>
+      </c>
+      <c r="C30" s="7">
+        <v>1336</v>
+      </c>
+      <c r="D30" s="7">
+        <v>513</v>
+      </c>
+      <c r="E30" s="7">
+        <v>165</v>
+      </c>
+      <c r="F30" s="7">
+        <v>109</v>
+      </c>
+      <c r="G30" s="7">
+        <v>926</v>
+      </c>
+      <c r="H30" s="7">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I30" s="7">
+        <v>4450</v>
+      </c>
+      <c r="J30" s="7">
+        <v>2983</v>
+      </c>
+      <c r="K30" s="7">
+        <v>1467</v>
+      </c>
+      <c r="L30" s="7">
+        <v>909</v>
+      </c>
+      <c r="M30" s="7">
+        <v>813</v>
+      </c>
+      <c r="N30" s="7">
+        <v>62</v>
+      </c>
+      <c r="O30" s="7">
+        <v>34</v>
+      </c>
+      <c r="P30" s="7">
+        <v>22.3</v>
+      </c>
+      <c r="Q30" s="7">
+        <v>25.81</v>
+      </c>
+      <c r="R30" s="7">
+        <v>16.829999999999998</v>
+      </c>
+      <c r="S30" s="7">
+        <v>29.81</v>
+      </c>
+      <c r="T30" s="7">
+        <v>26.66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="7">
+        <v>256</v>
+      </c>
+      <c r="C31" s="7">
+        <v>101</v>
+      </c>
+      <c r="D31" s="7">
+        <v>34</v>
+      </c>
+      <c r="E31" s="7">
+        <v>17</v>
+      </c>
+      <c r="F31" s="7">
+        <v>12</v>
+      </c>
+      <c r="G31" s="7">
+        <v>92</v>
+      </c>
+      <c r="H31" s="7">
+        <v>7.7</v>
+      </c>
+      <c r="I31" s="7">
+        <v>346</v>
+      </c>
+      <c r="J31" s="7">
+        <v>189</v>
+      </c>
+      <c r="K31" s="7">
+        <v>157</v>
+      </c>
+      <c r="L31" s="7">
+        <v>116</v>
+      </c>
+      <c r="M31" s="7">
+        <v>105</v>
+      </c>
+      <c r="N31" s="7">
+        <v>4</v>
+      </c>
+      <c r="O31" s="7">
+        <v>7</v>
+      </c>
+      <c r="P31" s="7">
+        <v>27</v>
+      </c>
+      <c r="Q31" s="7">
+        <v>24.61</v>
+      </c>
+      <c r="R31" s="7">
+        <v>13.28</v>
+      </c>
+      <c r="S31" s="7">
+        <v>45.31</v>
+      </c>
+      <c r="T31" s="7">
+        <v>41.02</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="7">
+        <v>18375</v>
+      </c>
+      <c r="C32" s="7">
+        <v>6431</v>
+      </c>
+      <c r="D32" s="7">
+        <v>3980</v>
+      </c>
+      <c r="E32" s="7">
+        <v>1276</v>
+      </c>
+      <c r="F32" s="7">
+        <v>828</v>
+      </c>
+      <c r="G32" s="7">
+        <v>5860</v>
+      </c>
+      <c r="H32" s="7">
+        <v>12.7</v>
+      </c>
+      <c r="I32" s="7">
+        <v>21781</v>
+      </c>
+      <c r="J32" s="7">
+        <v>13942</v>
+      </c>
+      <c r="K32" s="7">
+        <v>7839</v>
+      </c>
+      <c r="L32" s="7">
+        <v>4370</v>
+      </c>
+      <c r="M32" s="7">
+        <v>3686</v>
+      </c>
+      <c r="N32" s="7">
+        <v>455</v>
+      </c>
+      <c r="O32" s="7">
+        <v>229</v>
+      </c>
+      <c r="P32" s="7">
+        <v>19</v>
+      </c>
+      <c r="Q32" s="7">
+        <v>33.11</v>
+      </c>
+      <c r="R32" s="7">
+        <v>21.66</v>
+      </c>
+      <c r="S32" s="7">
+        <v>23.78</v>
+      </c>
+      <c r="T32" s="7">
+        <v>20.059999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="A33" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="7">
+        <v>2604</v>
+      </c>
+      <c r="C33" s="7">
+        <v>875</v>
+      </c>
+      <c r="D33" s="7">
+        <v>623</v>
+      </c>
+      <c r="E33" s="7">
+        <v>198</v>
+      </c>
+      <c r="F33" s="7">
+        <v>128</v>
+      </c>
+      <c r="G33" s="7">
+        <v>780</v>
+      </c>
+      <c r="H33" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I33" s="7">
+        <v>3441</v>
+      </c>
+      <c r="J33" s="7">
+        <v>2164</v>
+      </c>
+      <c r="K33" s="7">
+        <v>1277</v>
+      </c>
+      <c r="L33" s="7">
+        <v>809</v>
+      </c>
+      <c r="M33" s="7">
+        <v>717</v>
+      </c>
+      <c r="N33" s="7">
+        <v>65</v>
+      </c>
+      <c r="O33" s="7">
+        <v>27</v>
+      </c>
+      <c r="P33" s="7">
+        <v>23.7</v>
+      </c>
+      <c r="Q33" s="7">
+        <v>36.44</v>
+      </c>
+      <c r="R33" s="7">
+        <v>23.92</v>
+      </c>
+      <c r="S33" s="7">
+        <v>31.07</v>
+      </c>
+      <c r="T33" s="7">
+        <v>27.53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
+      <c r="A34" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="7">
+        <v>1267</v>
+      </c>
+      <c r="C34" s="7">
+        <v>631</v>
+      </c>
+      <c r="D34" s="7">
+        <v>103</v>
+      </c>
+      <c r="E34" s="7">
+        <v>69</v>
+      </c>
+      <c r="F34" s="7">
+        <v>47</v>
+      </c>
+      <c r="G34" s="7">
+        <v>417</v>
+      </c>
+      <c r="H34" s="7">
+        <v>11.3</v>
+      </c>
+      <c r="I34" s="7">
+        <v>1991</v>
+      </c>
+      <c r="J34" s="7">
+        <v>1191</v>
+      </c>
+      <c r="K34" s="7">
+        <v>800</v>
+      </c>
+      <c r="L34" s="7">
+        <v>583</v>
+      </c>
+      <c r="M34" s="7">
+        <v>509</v>
+      </c>
+      <c r="N34" s="7">
+        <v>58</v>
+      </c>
+      <c r="O34" s="7">
+        <v>16</v>
+      </c>
+      <c r="P34" s="7">
+        <v>30</v>
+      </c>
+      <c r="Q34" s="7">
+        <v>17.28</v>
+      </c>
+      <c r="R34" s="7">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="S34" s="7">
+        <v>46.01</v>
+      </c>
+      <c r="T34" s="7">
+        <v>40.17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20">
+      <c r="A35" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="7">
+        <v>353</v>
+      </c>
+      <c r="C35" s="7">
+        <v>176</v>
+      </c>
+      <c r="D35" s="7">
+        <v>35</v>
+      </c>
+      <c r="E35" s="7">
+        <v>19</v>
+      </c>
+      <c r="F35" s="7">
+        <v>16</v>
+      </c>
+      <c r="G35" s="7">
+        <v>107</v>
+      </c>
+      <c r="H35" s="7">
+        <v>16.3</v>
+      </c>
+      <c r="I35" s="7">
+        <v>486</v>
+      </c>
+      <c r="J35" s="7">
+        <v>278</v>
+      </c>
+      <c r="K35" s="7">
+        <v>208</v>
+      </c>
+      <c r="L35" s="7">
+        <v>103</v>
+      </c>
+      <c r="M35" s="7">
+        <v>93</v>
+      </c>
+      <c r="N35" s="7">
+        <v>8</v>
+      </c>
+      <c r="O35" s="7">
+        <v>2</v>
+      </c>
+      <c r="P35" s="7">
+        <v>29.7</v>
+      </c>
+      <c r="Q35" s="7">
+        <v>19.829999999999998</v>
+      </c>
+      <c r="R35" s="7">
+        <v>9.92</v>
+      </c>
+      <c r="S35" s="7">
+        <v>29.18</v>
+      </c>
+      <c r="T35" s="7">
+        <v>26.35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20">
+      <c r="A36" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="7">
+        <v>102770</v>
+      </c>
+      <c r="C36" s="7">
+        <v>57115</v>
+      </c>
+      <c r="D36" s="7">
+        <v>15673</v>
+      </c>
+      <c r="E36" s="7">
+        <v>5396</v>
+      </c>
+      <c r="F36" s="7">
+        <v>3121</v>
+      </c>
+      <c r="G36" s="7">
+        <v>21465</v>
+      </c>
+      <c r="H36" s="7">
+        <v>10</v>
+      </c>
+      <c r="I36" s="7">
+        <v>143695</v>
+      </c>
+      <c r="J36" s="7">
+        <v>83846</v>
+      </c>
+      <c r="K36" s="7">
+        <v>59849</v>
+      </c>
+      <c r="L36" s="7">
+        <v>29819</v>
+      </c>
+      <c r="M36" s="7">
+        <v>27209</v>
+      </c>
+      <c r="N36" s="7">
+        <v>1662</v>
+      </c>
+      <c r="O36" s="7">
+        <v>948</v>
+      </c>
+      <c r="P36" s="7">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="Q36" s="7">
+        <v>23.54</v>
+      </c>
+      <c r="R36" s="7">
+        <v>15.25</v>
+      </c>
+      <c r="S36" s="7">
+        <v>29.02</v>
+      </c>
+      <c r="T36" s="7">
+        <v>26.48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20">
+      <c r="A37" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="7">
+        <v>2610</v>
+      </c>
+      <c r="C37" s="7">
+        <v>936</v>
+      </c>
+      <c r="D37" s="7">
+        <v>548</v>
+      </c>
+      <c r="E37" s="7">
+        <v>184</v>
+      </c>
+      <c r="F37" s="7">
+        <v>118</v>
+      </c>
+      <c r="G37" s="7">
+        <v>824</v>
+      </c>
+      <c r="H37" s="7">
+        <v>11</v>
+      </c>
+      <c r="I37" s="7">
+        <v>4079</v>
+      </c>
+      <c r="J37" s="7">
+        <v>2690</v>
+      </c>
+      <c r="K37" s="7">
+        <v>1389</v>
+      </c>
+      <c r="L37" s="7">
+        <v>636</v>
+      </c>
+      <c r="M37" s="7">
+        <v>526</v>
+      </c>
+      <c r="N37" s="7">
+        <v>63</v>
+      </c>
+      <c r="O37" s="7">
+        <v>47</v>
+      </c>
+      <c r="P37" s="7">
+        <v>23</v>
+      </c>
+      <c r="Q37" s="7">
+        <v>32.57</v>
+      </c>
+      <c r="R37" s="7">
+        <v>21</v>
+      </c>
+      <c r="S37" s="7">
+        <v>24.37</v>
+      </c>
+      <c r="T37" s="7">
+        <v>20.149999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20">
+      <c r="A38" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="7">
+        <v>1434</v>
+      </c>
+      <c r="C38" s="7">
+        <v>733</v>
+      </c>
+      <c r="D38" s="7">
+        <v>184</v>
+      </c>
+      <c r="E38" s="7">
+        <v>94</v>
+      </c>
+      <c r="F38" s="7">
+        <v>51</v>
+      </c>
+      <c r="G38" s="7">
+        <v>372</v>
+      </c>
+      <c r="H38" s="7">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I38" s="7">
+        <v>1721</v>
+      </c>
+      <c r="J38" s="7">
+        <v>998</v>
+      </c>
+      <c r="K38" s="7">
+        <v>723</v>
+      </c>
+      <c r="L38" s="7">
+        <v>412</v>
+      </c>
+      <c r="M38" s="7">
+        <v>362</v>
+      </c>
+      <c r="N38" s="7">
+        <v>34</v>
+      </c>
+      <c r="O38" s="7">
+        <v>16</v>
+      </c>
+      <c r="P38" s="7">
+        <v>29</v>
+      </c>
+      <c r="Q38" s="7">
+        <v>22.94</v>
+      </c>
+      <c r="R38" s="7">
+        <v>12.83</v>
+      </c>
+      <c r="S38" s="7">
+        <v>28.73</v>
+      </c>
+      <c r="T38" s="7">
+        <v>25.24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20">
+      <c r="A39" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="7">
+        <v>236</v>
+      </c>
+      <c r="C39" s="7">
+        <v>110</v>
+      </c>
+      <c r="D39" s="7">
+        <v>34</v>
+      </c>
+      <c r="E39" s="7">
+        <v>14</v>
+      </c>
+      <c r="F39" s="7">
+        <v>9</v>
+      </c>
+      <c r="G39" s="7">
+        <v>69</v>
+      </c>
+      <c r="H39" s="7">
+        <v>18.7</v>
+      </c>
+      <c r="I39" s="7">
+        <v>351</v>
+      </c>
+      <c r="J39" s="7">
+        <v>168</v>
+      </c>
+      <c r="K39" s="7">
+        <v>183</v>
+      </c>
+      <c r="L39" s="7">
+        <v>57</v>
+      </c>
+      <c r="M39" s="7">
+        <v>44</v>
+      </c>
+      <c r="N39" s="7">
+        <v>9</v>
+      </c>
+      <c r="O39" s="7">
+        <v>4</v>
+      </c>
+      <c r="P39" s="7">
+        <v>23.7</v>
+      </c>
+      <c r="Q39" s="7">
+        <v>24.15</v>
+      </c>
+      <c r="R39" s="7">
+        <v>14.41</v>
+      </c>
+      <c r="S39" s="7">
+        <v>24.15</v>
+      </c>
+      <c r="T39" s="7">
+        <v>18.64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20">
+      <c r="A40" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="7">
+        <v>1340</v>
+      </c>
+      <c r="C40" s="7">
+        <v>530</v>
+      </c>
+      <c r="D40" s="7">
+        <v>224</v>
+      </c>
+      <c r="E40" s="7">
+        <v>99</v>
+      </c>
+      <c r="F40" s="7">
+        <v>54</v>
+      </c>
+      <c r="G40" s="7">
+        <v>433</v>
+      </c>
+      <c r="H40" s="7">
+        <v>11.7</v>
+      </c>
+      <c r="I40" s="7">
+        <v>1886</v>
+      </c>
+      <c r="J40" s="7">
+        <v>1032</v>
+      </c>
+      <c r="K40" s="7">
+        <v>854</v>
+      </c>
+      <c r="L40" s="7">
+        <v>508</v>
+      </c>
+      <c r="M40" s="7">
+        <v>400</v>
+      </c>
+      <c r="N40" s="7">
+        <v>71</v>
+      </c>
+      <c r="O40" s="7">
+        <v>37</v>
+      </c>
+      <c r="P40" s="7">
+        <v>29.7</v>
+      </c>
+      <c r="Q40" s="7">
+        <v>28.13</v>
+      </c>
+      <c r="R40" s="7">
+        <v>16.72</v>
+      </c>
+      <c r="S40" s="7">
+        <v>37.909999999999997</v>
+      </c>
+      <c r="T40" s="7">
+        <v>29.85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20">
+      <c r="A41" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="7">
+        <v>5349</v>
+      </c>
+      <c r="C41" s="7">
+        <v>1804</v>
+      </c>
+      <c r="D41" s="7">
+        <v>1066</v>
+      </c>
+      <c r="E41" s="7">
+        <v>398</v>
+      </c>
+      <c r="F41" s="7">
+        <v>278</v>
+      </c>
+      <c r="G41" s="7">
+        <v>1803</v>
+      </c>
+      <c r="H41" s="7">
+        <v>16</v>
+      </c>
+      <c r="I41" s="7">
+        <v>7567</v>
+      </c>
+      <c r="J41" s="7">
+        <v>4993</v>
+      </c>
+      <c r="K41" s="7">
+        <v>2574</v>
+      </c>
+      <c r="L41" s="7">
+        <v>1766</v>
+      </c>
+      <c r="M41" s="7">
+        <v>1584</v>
+      </c>
+      <c r="N41" s="7">
+        <v>107</v>
+      </c>
+      <c r="O41" s="7">
+        <v>75</v>
+      </c>
+      <c r="P41" s="7">
+        <v>25</v>
+      </c>
+      <c r="Q41" s="7">
+        <v>32.57</v>
+      </c>
+      <c r="R41" s="7">
+        <v>19.93</v>
+      </c>
+      <c r="S41" s="7">
+        <v>33.020000000000003</v>
+      </c>
+      <c r="T41" s="7">
+        <v>29.61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20">
+      <c r="A42" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="7">
+        <v>139</v>
+      </c>
+      <c r="C42" s="7">
+        <v>67</v>
+      </c>
+      <c r="D42" s="7">
+        <v>24</v>
+      </c>
+      <c r="E42" s="7">
+        <v>9</v>
+      </c>
+      <c r="F42" s="7">
+        <v>8</v>
+      </c>
+      <c r="G42" s="7">
+        <v>31</v>
+      </c>
+      <c r="H42" s="7">
+        <v>12</v>
+      </c>
+      <c r="I42" s="7">
+        <v>168</v>
+      </c>
+      <c r="J42" s="7">
+        <v>83</v>
+      </c>
+      <c r="K42" s="7">
+        <v>85</v>
+      </c>
+      <c r="L42" s="7">
+        <v>50</v>
+      </c>
+      <c r="M42" s="7">
+        <v>44</v>
+      </c>
+      <c r="N42" s="7">
+        <v>3</v>
+      </c>
+      <c r="O42" s="7">
+        <v>3</v>
+      </c>
+      <c r="P42" s="7">
+        <v>24</v>
+      </c>
+      <c r="Q42" s="7">
+        <v>29.5</v>
+      </c>
+      <c r="R42" s="7">
+        <v>17.27</v>
+      </c>
+      <c r="S42" s="7">
+        <v>35.97</v>
+      </c>
+      <c r="T42" s="7">
+        <v>31.65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20">
+      <c r="A43" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="7">
+        <v>180</v>
+      </c>
+      <c r="C43" s="7">
+        <v>108</v>
+      </c>
+      <c r="D43" s="7">
+        <v>9</v>
+      </c>
+      <c r="E43" s="7">
+        <v>4</v>
+      </c>
+      <c r="F43" s="7">
+        <v>7</v>
+      </c>
+      <c r="G43" s="7">
+        <v>52</v>
+      </c>
+      <c r="H43" s="7">
+        <v>10.7</v>
+      </c>
+      <c r="I43" s="7">
+        <v>157</v>
+      </c>
+      <c r="J43" s="7">
+        <v>68</v>
+      </c>
+      <c r="K43" s="7">
+        <v>89</v>
+      </c>
+      <c r="L43" s="7">
+        <v>20</v>
+      </c>
+      <c r="M43" s="7">
+        <v>16</v>
+      </c>
+      <c r="N43" s="7">
+        <v>2</v>
+      </c>
+      <c r="O43" s="7">
+        <v>2</v>
+      </c>
+      <c r="P43" s="7">
+        <v>24.7</v>
+      </c>
+      <c r="Q43" s="7">
+        <v>11.11</v>
+      </c>
+      <c r="R43" s="7">
+        <v>5</v>
+      </c>
+      <c r="S43" s="7">
+        <v>11.11</v>
+      </c>
+      <c r="T43" s="7">
+        <v>8.89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20">
+      <c r="A44" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="7">
+        <v>8815</v>
+      </c>
+      <c r="C44" s="7">
+        <v>2272</v>
+      </c>
+      <c r="D44" s="7">
+        <v>1574</v>
+      </c>
+      <c r="E44" s="7">
+        <v>747</v>
+      </c>
+      <c r="F44" s="7">
+        <v>504</v>
+      </c>
+      <c r="G44" s="7">
+        <v>3718</v>
+      </c>
+      <c r="H44" s="7">
+        <v>15.3</v>
+      </c>
+      <c r="I44" s="7">
+        <v>9966</v>
+      </c>
+      <c r="J44" s="7">
+        <v>5988</v>
+      </c>
+      <c r="K44" s="7">
+        <v>3978</v>
+      </c>
+      <c r="L44" s="7">
+        <v>2681</v>
+      </c>
+      <c r="M44" s="7">
+        <v>2299</v>
+      </c>
+      <c r="N44" s="7">
+        <v>282</v>
+      </c>
+      <c r="O44" s="7">
+        <v>100</v>
+      </c>
+      <c r="P44" s="7">
+        <v>24.7</v>
+      </c>
+      <c r="Q44" s="7">
+        <v>32.049999999999997</v>
+      </c>
+      <c r="R44" s="7">
+        <v>17.86</v>
+      </c>
+      <c r="S44" s="7">
+        <v>30.41</v>
+      </c>
+      <c r="T44" s="7">
+        <v>26.08</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20">
+      <c r="A45" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" s="7">
+        <v>852</v>
+      </c>
+      <c r="C45" s="7">
+        <v>373</v>
+      </c>
+      <c r="D45" s="7">
+        <v>116</v>
+      </c>
+      <c r="E45" s="7">
+        <v>44</v>
+      </c>
+      <c r="F45" s="7">
+        <v>36</v>
+      </c>
+      <c r="G45" s="7">
+        <v>283</v>
+      </c>
+      <c r="H45" s="7">
+        <v>14.7</v>
+      </c>
+      <c r="I45" s="7">
+        <v>1212</v>
+      </c>
+      <c r="J45" s="7">
+        <v>664</v>
+      </c>
+      <c r="K45" s="7">
+        <v>548</v>
+      </c>
+      <c r="L45" s="7">
+        <v>268</v>
+      </c>
+      <c r="M45" s="7">
+        <v>221</v>
+      </c>
+      <c r="N45" s="7">
+        <v>33</v>
+      </c>
+      <c r="O45" s="7">
+        <v>14</v>
+      </c>
+      <c r="P45" s="7">
+        <v>24.3</v>
+      </c>
+      <c r="Q45" s="7">
+        <v>23</v>
+      </c>
+      <c r="R45" s="7">
+        <v>13.62</v>
+      </c>
+      <c r="S45" s="7">
+        <v>31.46</v>
+      </c>
+      <c r="T45" s="7">
+        <v>25.94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20">
+      <c r="A46" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="7">
+        <v>1051</v>
+      </c>
+      <c r="C46" s="7">
+        <v>543</v>
+      </c>
+      <c r="D46" s="7">
+        <v>99</v>
+      </c>
+      <c r="E46" s="7">
+        <v>55</v>
+      </c>
+      <c r="F46" s="7">
+        <v>42</v>
+      </c>
+      <c r="G46" s="7">
+        <v>312</v>
+      </c>
+      <c r="H46" s="7">
+        <v>15.7</v>
+      </c>
+      <c r="I46" s="7">
+        <v>1199</v>
+      </c>
+      <c r="J46" s="7">
+        <v>612</v>
+      </c>
+      <c r="K46" s="7">
+        <v>587</v>
+      </c>
+      <c r="L46" s="7">
+        <v>253</v>
+      </c>
+      <c r="M46" s="7">
+        <v>211</v>
+      </c>
+      <c r="N46" s="7">
+        <v>30</v>
+      </c>
+      <c r="O46" s="7">
+        <v>12</v>
+      </c>
+      <c r="P46" s="7">
+        <v>25.7</v>
+      </c>
+      <c r="Q46" s="7">
+        <v>18.649999999999999</v>
+      </c>
+      <c r="R46" s="7">
+        <v>9.42</v>
+      </c>
+      <c r="S46" s="7">
+        <v>24.07</v>
+      </c>
+      <c r="T46" s="7">
+        <v>20.079999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20">
+      <c r="A47" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="7">
+        <v>23220</v>
+      </c>
+      <c r="C47" s="7">
+        <v>11313</v>
+      </c>
+      <c r="D47" s="7">
+        <v>2682</v>
+      </c>
+      <c r="E47" s="7">
+        <v>1494</v>
+      </c>
+      <c r="F47" s="7">
+        <v>926</v>
+      </c>
+      <c r="G47" s="7">
+        <v>6805</v>
+      </c>
+      <c r="H47" s="7">
+        <v>5.7</v>
+      </c>
+      <c r="I47" s="7">
+        <v>26310</v>
+      </c>
+      <c r="J47" s="7">
+        <v>20817</v>
+      </c>
+      <c r="K47" s="7">
+        <v>5493</v>
+      </c>
+      <c r="L47" s="7">
+        <v>3051</v>
+      </c>
+      <c r="M47" s="7">
+        <v>2016</v>
+      </c>
+      <c r="N47" s="7">
+        <v>602</v>
+      </c>
+      <c r="O47" s="7">
+        <v>433</v>
+      </c>
+      <c r="P47" s="7">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="Q47" s="7">
+        <v>21.97</v>
+      </c>
+      <c r="R47" s="7">
+        <v>11.55</v>
+      </c>
+      <c r="S47" s="7">
+        <v>13.14</v>
+      </c>
+      <c r="T47" s="7">
+        <v>8.68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20">
+      <c r="A48" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" s="7">
+        <v>2660</v>
+      </c>
+      <c r="C48" s="7">
+        <v>1364</v>
+      </c>
+      <c r="D48" s="7">
+        <v>276</v>
+      </c>
+      <c r="E48" s="7">
+        <v>141</v>
+      </c>
+      <c r="F48" s="7">
+        <v>93</v>
+      </c>
+      <c r="G48" s="7">
+        <v>786</v>
+      </c>
+      <c r="H48" s="7">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I48" s="7">
+        <v>2011</v>
+      </c>
+      <c r="J48" s="7">
+        <v>1449</v>
+      </c>
+      <c r="K48" s="7">
+        <v>562</v>
+      </c>
+      <c r="L48" s="7">
+        <v>323</v>
+      </c>
+      <c r="M48" s="7">
+        <v>204</v>
+      </c>
+      <c r="N48" s="7">
+        <v>65</v>
+      </c>
+      <c r="O48" s="7">
+        <v>54</v>
+      </c>
+      <c r="P48" s="7">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="Q48" s="7">
+        <v>19.170000000000002</v>
+      </c>
+      <c r="R48" s="7">
+        <v>10.38</v>
+      </c>
+      <c r="S48" s="7">
+        <v>12.14</v>
+      </c>
+      <c r="T48" s="7">
+        <v>7.67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20">
+      <c r="A49" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B49" s="7">
+        <v>314</v>
+      </c>
+      <c r="C49" s="7">
+        <v>167</v>
+      </c>
+      <c r="D49" s="7">
+        <v>28</v>
+      </c>
+      <c r="E49" s="7">
+        <v>17</v>
+      </c>
+      <c r="F49" s="7">
+        <v>8</v>
+      </c>
+      <c r="G49" s="7">
+        <v>94</v>
+      </c>
+      <c r="H49" s="7">
+        <v>15.3</v>
+      </c>
+      <c r="I49" s="7">
+        <v>414</v>
+      </c>
+      <c r="J49" s="7">
+        <v>209</v>
+      </c>
+      <c r="K49" s="7">
+        <v>205</v>
+      </c>
+      <c r="L49" s="7">
+        <v>86</v>
+      </c>
+      <c r="M49" s="7">
+        <v>78</v>
+      </c>
+      <c r="N49" s="7">
+        <v>6</v>
+      </c>
+      <c r="O49" s="7">
+        <v>2</v>
+      </c>
+      <c r="P49" s="7">
+        <v>27.7</v>
+      </c>
+      <c r="Q49" s="7">
+        <v>16.88</v>
+      </c>
+      <c r="R49" s="7">
+        <v>8.92</v>
+      </c>
+      <c r="S49" s="7">
+        <v>27.39</v>
+      </c>
+      <c r="T49" s="7">
+        <v>24.84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20">
+      <c r="A50" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="7">
+        <v>29264</v>
+      </c>
+      <c r="C50" s="7">
+        <v>12314</v>
+      </c>
+      <c r="D50" s="7">
+        <v>5294</v>
+      </c>
+      <c r="E50" s="7">
+        <v>1921</v>
+      </c>
+      <c r="F50" s="7">
+        <v>1118</v>
+      </c>
+      <c r="G50" s="7">
+        <v>8617</v>
+      </c>
+      <c r="H50" s="7">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I50" s="7">
+        <v>35556</v>
+      </c>
+      <c r="J50" s="7">
+        <v>21304</v>
+      </c>
+      <c r="K50" s="7">
+        <v>14252</v>
+      </c>
+      <c r="L50" s="7">
+        <v>6883</v>
+      </c>
+      <c r="M50" s="7">
+        <v>5789</v>
+      </c>
+      <c r="N50" s="7">
+        <v>719</v>
+      </c>
+      <c r="O50" s="7">
+        <v>375</v>
+      </c>
+      <c r="P50" s="7">
+        <v>24.7</v>
+      </c>
+      <c r="Q50" s="7">
+        <v>28.48</v>
+      </c>
+      <c r="R50" s="7">
+        <v>18.09</v>
+      </c>
+      <c r="S50" s="7">
+        <v>23.52</v>
+      </c>
+      <c r="T50" s="7">
+        <v>19.78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20">
+      <c r="A51" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="7">
+        <v>22587</v>
+      </c>
+      <c r="C51" s="7">
+        <v>10348</v>
+      </c>
+      <c r="D51" s="7">
+        <v>2936</v>
+      </c>
+      <c r="E51" s="7">
+        <v>1517</v>
+      </c>
+      <c r="F51" s="7">
+        <v>877</v>
+      </c>
+      <c r="G51" s="7">
+        <v>6909</v>
+      </c>
+      <c r="H51" s="7">
+        <v>7</v>
+      </c>
+      <c r="I51" s="7">
+        <v>22055</v>
+      </c>
+      <c r="J51" s="7">
+        <v>17406</v>
+      </c>
+      <c r="K51" s="7">
+        <v>4649</v>
+      </c>
+      <c r="L51" s="7">
+        <v>3074</v>
+      </c>
+      <c r="M51" s="7">
+        <v>2052</v>
+      </c>
+      <c r="N51" s="7">
+        <v>601</v>
+      </c>
+      <c r="O51" s="7">
+        <v>421</v>
+      </c>
+      <c r="P51" s="7">
+        <v>35</v>
+      </c>
+      <c r="Q51" s="7">
+        <v>23.6</v>
+      </c>
+      <c r="R51" s="7">
+        <v>13</v>
+      </c>
+      <c r="S51" s="7">
+        <v>13.61</v>
+      </c>
+      <c r="T51" s="7">
+        <v>9.08</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20">
+      <c r="A52" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B52" s="7">
+        <v>587</v>
+      </c>
+      <c r="C52" s="7">
+        <v>241</v>
+      </c>
+      <c r="D52" s="7">
+        <v>89</v>
+      </c>
+      <c r="E52" s="7">
+        <v>39</v>
+      </c>
+      <c r="F52" s="7">
+        <v>24</v>
+      </c>
+      <c r="G52" s="7">
+        <v>194</v>
+      </c>
+      <c r="H52" s="7">
+        <v>17.7</v>
+      </c>
+      <c r="I52" s="7">
+        <v>912</v>
+      </c>
+      <c r="J52" s="7">
+        <v>508</v>
+      </c>
+      <c r="K52" s="7">
+        <v>404</v>
+      </c>
+      <c r="L52" s="7">
+        <v>258</v>
+      </c>
+      <c r="M52" s="7">
+        <v>229</v>
+      </c>
+      <c r="N52" s="7">
+        <v>25</v>
+      </c>
+      <c r="O52" s="7">
+        <v>4</v>
+      </c>
+      <c r="P52" s="7">
+        <v>25.7</v>
+      </c>
+      <c r="Q52" s="7">
+        <v>25.89</v>
+      </c>
+      <c r="R52" s="7">
+        <v>15.16</v>
+      </c>
+      <c r="S52" s="7">
+        <v>43.95</v>
+      </c>
+      <c r="T52" s="7">
+        <v>39.01</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20">
+      <c r="A53" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" s="7">
+        <v>34698</v>
+      </c>
+      <c r="C53" s="7">
+        <v>12420</v>
+      </c>
+      <c r="D53" s="7">
+        <v>8340</v>
+      </c>
+      <c r="E53" s="7">
+        <v>2422</v>
+      </c>
+      <c r="F53" s="7">
+        <v>1324</v>
+      </c>
+      <c r="G53" s="7">
+        <v>10192</v>
+      </c>
+      <c r="H53" s="7">
+        <v>8</v>
+      </c>
+      <c r="I53" s="7">
+        <v>47679</v>
+      </c>
+      <c r="J53" s="7">
+        <v>29483</v>
+      </c>
+      <c r="K53" s="7">
+        <v>18196</v>
+      </c>
+      <c r="L53" s="7">
+        <v>11777</v>
+      </c>
+      <c r="M53" s="7">
+        <v>10382</v>
+      </c>
+      <c r="N53" s="7">
+        <v>909</v>
+      </c>
+      <c r="O53" s="7">
+        <v>486</v>
+      </c>
+      <c r="P53" s="7">
+        <v>28.7</v>
+      </c>
+      <c r="Q53" s="7">
+        <v>34.83</v>
+      </c>
+      <c r="R53" s="7">
+        <v>24.04</v>
+      </c>
+      <c r="S53" s="7">
+        <v>33.94</v>
+      </c>
+      <c r="T53" s="7">
+        <v>29.92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20">
+      <c r="A54" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" s="7">
+        <v>39805</v>
+      </c>
+      <c r="C54" s="7">
+        <v>17811</v>
+      </c>
+      <c r="D54" s="7">
+        <v>5203</v>
+      </c>
+      <c r="E54" s="7">
+        <v>2543</v>
+      </c>
+      <c r="F54" s="7">
+        <v>1571</v>
+      </c>
+      <c r="G54" s="7">
+        <v>12677</v>
+      </c>
+      <c r="H54" s="7">
+        <v>12</v>
+      </c>
+      <c r="I54" s="7">
+        <v>31077</v>
+      </c>
+      <c r="J54" s="7">
+        <v>23446</v>
+      </c>
+      <c r="K54" s="7">
+        <v>7631</v>
+      </c>
+      <c r="L54" s="7">
+        <v>4832</v>
+      </c>
+      <c r="M54" s="7">
+        <v>2952</v>
+      </c>
+      <c r="N54" s="7">
+        <v>1101</v>
+      </c>
+      <c r="O54" s="7">
+        <v>779</v>
+      </c>
+      <c r="P54" s="7">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="Q54" s="7">
+        <v>23.41</v>
+      </c>
+      <c r="R54" s="7">
+        <v>13.07</v>
+      </c>
+      <c r="S54" s="7">
+        <v>12.14</v>
+      </c>
+      <c r="T54" s="7">
+        <v>7.42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20">
+      <c r="A55" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" s="7">
+        <v>7885</v>
+      </c>
+      <c r="C55" s="7">
+        <v>4017</v>
+      </c>
+      <c r="D55" s="7">
+        <v>845</v>
+      </c>
+      <c r="E55" s="7">
+        <v>472</v>
+      </c>
+      <c r="F55" s="7">
+        <v>337</v>
+      </c>
+      <c r="G55" s="7">
+        <v>2214</v>
+      </c>
+      <c r="H55" s="7">
+        <v>7.7</v>
+      </c>
+      <c r="I55" s="7">
+        <v>6422</v>
+      </c>
+      <c r="J55" s="7">
+        <v>4750</v>
+      </c>
+      <c r="K55" s="7">
+        <v>1672</v>
+      </c>
+      <c r="L55" s="7">
+        <v>1095</v>
+      </c>
+      <c r="M55" s="7">
+        <v>752</v>
+      </c>
+      <c r="N55" s="7">
+        <v>205</v>
+      </c>
+      <c r="O55" s="7">
+        <v>138</v>
+      </c>
+      <c r="P55" s="7">
+        <v>34</v>
+      </c>
+      <c r="Q55" s="7">
+        <v>20.98</v>
+      </c>
+      <c r="R55" s="7">
+        <v>10.72</v>
+      </c>
+      <c r="S55" s="7">
+        <v>13.89</v>
+      </c>
+      <c r="T55" s="7">
+        <v>9.5399999999999991</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20">
+      <c r="A56" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B56" s="7">
+        <v>9670</v>
+      </c>
+      <c r="C56" s="7">
+        <v>4014</v>
+      </c>
+      <c r="D56" s="7">
+        <v>1819</v>
+      </c>
+      <c r="E56" s="7">
+        <v>604</v>
+      </c>
+      <c r="F56" s="7">
+        <v>364</v>
+      </c>
+      <c r="G56" s="7">
+        <v>2869</v>
+      </c>
+      <c r="H56" s="7">
+        <v>12</v>
+      </c>
+      <c r="I56" s="7">
+        <v>14912</v>
+      </c>
+      <c r="J56" s="7">
+        <v>9604</v>
+      </c>
+      <c r="K56" s="7">
+        <v>5308</v>
+      </c>
+      <c r="L56" s="7">
+        <v>3298</v>
+      </c>
+      <c r="M56" s="7">
+        <v>2915</v>
+      </c>
+      <c r="N56" s="7">
+        <v>262</v>
+      </c>
+      <c r="O56" s="7">
+        <v>121</v>
+      </c>
+      <c r="P56" s="7">
+        <v>24.3</v>
+      </c>
+      <c r="Q56" s="7">
+        <v>28.82</v>
+      </c>
+      <c r="R56" s="7">
+        <v>18.809999999999999</v>
+      </c>
+      <c r="S56" s="7">
+        <v>34.11</v>
+      </c>
+      <c r="T56" s="7">
+        <v>30.14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20">
+      <c r="A57" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B57" s="7">
+        <v>2494</v>
+      </c>
+      <c r="C57" s="7">
+        <v>1161</v>
+      </c>
+      <c r="D57" s="7">
+        <v>220</v>
+      </c>
+      <c r="E57" s="7">
+        <v>155</v>
+      </c>
+      <c r="F57" s="7">
+        <v>103</v>
+      </c>
+      <c r="G57" s="7">
+        <v>855</v>
+      </c>
+      <c r="H57" s="7">
+        <v>10.7</v>
+      </c>
+      <c r="I57" s="7">
+        <v>2199</v>
+      </c>
+      <c r="J57" s="7">
+        <v>1687</v>
+      </c>
+      <c r="K57" s="7">
+        <v>512</v>
+      </c>
+      <c r="L57" s="7">
+        <v>250</v>
+      </c>
+      <c r="M57" s="7">
+        <v>146</v>
+      </c>
+      <c r="N57" s="7">
+        <v>63</v>
+      </c>
+      <c r="O57" s="7">
+        <v>41</v>
+      </c>
+      <c r="P57" s="7">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="Q57" s="7">
+        <v>19.170000000000002</v>
+      </c>
+      <c r="R57" s="7">
+        <v>8.82</v>
+      </c>
+      <c r="S57" s="7">
+        <v>10.02</v>
+      </c>
+      <c r="T57" s="7">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20">
+      <c r="A58" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B58" s="7">
+        <v>3639</v>
+      </c>
+      <c r="C58" s="7">
+        <v>1740</v>
+      </c>
+      <c r="D58" s="7">
+        <v>358</v>
+      </c>
+      <c r="E58" s="7">
+        <v>232</v>
+      </c>
+      <c r="F58" s="7">
+        <v>159</v>
+      </c>
+      <c r="G58" s="7">
+        <v>1150</v>
+      </c>
+      <c r="H58" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I58" s="7">
+        <v>3018</v>
+      </c>
+      <c r="J58" s="7">
+        <v>2278</v>
+      </c>
+      <c r="K58" s="7">
+        <v>740</v>
+      </c>
+      <c r="L58" s="7">
+        <v>435</v>
+      </c>
+      <c r="M58" s="7">
+        <v>255</v>
+      </c>
+      <c r="N58" s="7">
+        <v>100</v>
+      </c>
+      <c r="O58" s="7">
+        <v>80</v>
+      </c>
+      <c r="P58" s="7">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="Q58" s="7">
+        <v>20.58</v>
+      </c>
+      <c r="R58" s="7">
+        <v>9.84</v>
+      </c>
+      <c r="S58" s="7">
+        <v>11.95</v>
+      </c>
+      <c r="T58" s="7">
+        <v>7.01</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20">
+      <c r="A59" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B59" s="7">
+        <v>5850</v>
+      </c>
+      <c r="C59" s="7">
+        <v>2498</v>
+      </c>
+      <c r="D59" s="7">
+        <v>477</v>
+      </c>
+      <c r="E59" s="7">
+        <v>369</v>
+      </c>
+      <c r="F59" s="7">
+        <v>264</v>
+      </c>
+      <c r="G59" s="7">
+        <v>2242</v>
+      </c>
+      <c r="H59" s="7">
+        <v>15</v>
+      </c>
+      <c r="I59" s="7">
+        <v>4663</v>
+      </c>
+      <c r="J59" s="7">
+        <v>3768</v>
+      </c>
+      <c r="K59" s="7">
+        <v>895</v>
+      </c>
+      <c r="L59" s="7">
+        <v>592</v>
+      </c>
+      <c r="M59" s="7">
+        <v>341</v>
+      </c>
+      <c r="N59" s="7">
+        <v>155</v>
+      </c>
+      <c r="O59" s="7">
+        <v>96</v>
+      </c>
+      <c r="P59" s="7">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="Q59" s="7">
+        <v>18.97</v>
+      </c>
+      <c r="R59" s="7">
+        <v>8.15</v>
+      </c>
+      <c r="S59" s="7">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="T59" s="7">
+        <v>5.83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20">
+      <c r="A60" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B60" s="7">
+        <v>8849</v>
+      </c>
+      <c r="C60" s="7">
+        <v>4613</v>
+      </c>
+      <c r="D60" s="7">
+        <v>186</v>
+      </c>
+      <c r="E60" s="7">
+        <v>593</v>
+      </c>
+      <c r="F60" s="7">
+        <v>395</v>
+      </c>
+      <c r="G60" s="7">
+        <v>3062</v>
+      </c>
+      <c r="H60" s="7">
+        <v>7.7</v>
+      </c>
+      <c r="I60" s="7">
+        <v>11008</v>
+      </c>
+      <c r="J60" s="7">
+        <v>9011</v>
+      </c>
+      <c r="K60" s="7">
+        <v>1997</v>
+      </c>
+      <c r="L60" s="7">
+        <v>376</v>
+      </c>
+      <c r="M60" s="7">
+        <v>72</v>
+      </c>
+      <c r="N60" s="7">
+        <v>188</v>
+      </c>
+      <c r="O60" s="7">
+        <v>116</v>
+      </c>
+      <c r="P60" s="7">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="Q60" s="7">
+        <v>13.27</v>
+      </c>
+      <c r="R60" s="7">
+        <v>2.1</v>
+      </c>
+      <c r="S60" s="7">
+        <v>4.25</v>
+      </c>
+      <c r="T60" s="7">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20">
+      <c r="A61" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B61" s="7">
+        <v>3453</v>
+      </c>
+      <c r="C61" s="7">
+        <v>1594</v>
+      </c>
+      <c r="D61" s="7">
+        <v>82</v>
+      </c>
+      <c r="E61" s="7">
+        <v>213</v>
+      </c>
+      <c r="F61" s="7">
+        <v>172</v>
+      </c>
+      <c r="G61" s="7">
+        <v>1392</v>
+      </c>
+      <c r="H61" s="7">
+        <v>11</v>
+      </c>
+      <c r="I61" s="7">
+        <v>3367</v>
+      </c>
+      <c r="J61" s="7">
+        <v>2711</v>
+      </c>
+      <c r="K61" s="7">
+        <v>656</v>
+      </c>
+      <c r="L61" s="7">
+        <v>151</v>
+      </c>
+      <c r="M61" s="7">
+        <v>23</v>
+      </c>
+      <c r="N61" s="7">
+        <v>74</v>
+      </c>
+      <c r="O61" s="7">
+        <v>54</v>
+      </c>
+      <c r="P61" s="7">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="Q61" s="7">
+        <v>13.52</v>
+      </c>
+      <c r="R61" s="7">
+        <v>2.37</v>
+      </c>
+      <c r="S61" s="7">
+        <v>4.37</v>
+      </c>
+      <c r="T61" s="7">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20">
+      <c r="A62" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B62" s="7">
+        <v>3126</v>
+      </c>
+      <c r="C62" s="7">
+        <v>1228</v>
+      </c>
+      <c r="D62" s="7">
+        <v>549</v>
+      </c>
+      <c r="E62" s="7">
+        <v>212</v>
+      </c>
+      <c r="F62" s="7">
+        <v>128</v>
+      </c>
+      <c r="G62" s="7">
+        <v>1009</v>
+      </c>
+      <c r="H62" s="7">
+        <v>14.3</v>
+      </c>
+      <c r="I62" s="7">
+        <v>3697</v>
+      </c>
+      <c r="J62" s="7">
+        <v>2052</v>
+      </c>
+      <c r="K62" s="7">
+        <v>1645</v>
+      </c>
+      <c r="L62" s="7">
+        <v>1090</v>
+      </c>
+      <c r="M62" s="7">
+        <v>952</v>
+      </c>
+      <c r="N62" s="7">
+        <v>93</v>
+      </c>
+      <c r="O62" s="7">
+        <v>45</v>
+      </c>
+      <c r="P62" s="7">
+        <v>27.7</v>
+      </c>
+      <c r="Q62" s="7">
+        <v>28.44</v>
+      </c>
+      <c r="R62" s="7">
+        <v>17.559999999999999</v>
+      </c>
+      <c r="S62" s="7">
+        <v>34.869999999999997</v>
+      </c>
+      <c r="T62" s="7">
+        <v>30.45</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20">
+      <c r="A63" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B63" s="7">
+        <v>29</v>
+      </c>
+      <c r="C63" s="7">
+        <v>14</v>
+      </c>
+      <c r="D63" s="7">
+        <v>2</v>
+      </c>
+      <c r="E63" s="7">
+        <v>3</v>
+      </c>
+      <c r="F63" s="7">
+        <v>1</v>
+      </c>
+      <c r="G63" s="7">
+        <v>9</v>
+      </c>
+      <c r="H63" s="7">
+        <v>10.3</v>
+      </c>
+      <c r="I63" s="7">
+        <v>44</v>
+      </c>
+      <c r="J63" s="7">
+        <v>26</v>
+      </c>
+      <c r="K63" s="7">
+        <v>18</v>
+      </c>
+      <c r="L63" s="7">
+        <v>5</v>
+      </c>
+      <c r="M63" s="7">
+        <v>5</v>
+      </c>
+      <c r="N63" s="7">
+        <v>0</v>
+      </c>
+      <c r="O63" s="7">
+        <v>0</v>
+      </c>
+      <c r="P63" s="7">
+        <v>27</v>
+      </c>
+      <c r="Q63" s="7">
+        <v>20.69</v>
+      </c>
+      <c r="R63" s="7">
+        <v>6.9</v>
+      </c>
+      <c r="S63" s="7">
+        <v>17.239999999999998</v>
+      </c>
+      <c r="T63" s="7">
+        <v>17.239999999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20">
+      <c r="A64" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B64" s="7">
+        <v>824</v>
+      </c>
+      <c r="C64" s="7">
+        <v>403</v>
+      </c>
+      <c r="D64" s="7">
+        <v>117</v>
+      </c>
+      <c r="E64" s="7">
+        <v>49</v>
+      </c>
+      <c r="F64" s="7">
+        <v>28</v>
+      </c>
+      <c r="G64" s="7">
+        <v>227</v>
+      </c>
+      <c r="H64" s="7">
+        <v>20.7</v>
+      </c>
+      <c r="I64" s="7">
+        <v>1010</v>
+      </c>
+      <c r="J64" s="7">
+        <v>596</v>
+      </c>
+      <c r="K64" s="7">
+        <v>414</v>
+      </c>
+      <c r="L64" s="7">
+        <v>323</v>
+      </c>
+      <c r="M64" s="7">
+        <v>287</v>
+      </c>
+      <c r="N64" s="7">
+        <v>25</v>
+      </c>
+      <c r="O64" s="7">
+        <v>11</v>
+      </c>
+      <c r="P64" s="7">
+        <v>28.3</v>
+      </c>
+      <c r="Q64" s="7">
+        <v>23.54</v>
+      </c>
+      <c r="R64" s="7">
+        <v>14.2</v>
+      </c>
+      <c r="S64" s="7">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="T64" s="7">
+        <v>34.83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20">
+      <c r="A65" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B65" s="7">
+        <v>4566</v>
+      </c>
+      <c r="C65" s="7">
+        <v>2313</v>
+      </c>
+      <c r="D65" s="7">
+        <v>65</v>
+      </c>
+      <c r="E65" s="7">
+        <v>305</v>
+      </c>
+      <c r="F65" s="7">
+        <v>188</v>
+      </c>
+      <c r="G65" s="7">
+        <v>1695</v>
+      </c>
+      <c r="H65" s="7">
+        <v>11.3</v>
+      </c>
+      <c r="I65" s="7">
+        <v>4977</v>
+      </c>
+      <c r="J65" s="7">
+        <v>3759</v>
+      </c>
+      <c r="K65" s="7">
+        <v>1218</v>
+      </c>
+      <c r="L65" s="7">
+        <v>240</v>
+      </c>
+      <c r="M65" s="7">
+        <v>37</v>
+      </c>
+      <c r="N65" s="7">
+        <v>120</v>
+      </c>
+      <c r="O65" s="7">
+        <v>83</v>
+      </c>
+      <c r="P65" s="7">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="Q65" s="7">
+        <v>12.22</v>
+      </c>
+      <c r="R65" s="7">
+        <v>1.42</v>
+      </c>
+      <c r="S65" s="7">
+        <v>5.26</v>
+      </c>
+      <c r="T65" s="7">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20">
+      <c r="A66" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B66" s="7">
+        <v>4603</v>
+      </c>
+      <c r="C66" s="7">
+        <v>1850</v>
+      </c>
+      <c r="D66" s="7">
+        <v>572</v>
+      </c>
+      <c r="E66" s="7">
+        <v>324</v>
+      </c>
+      <c r="F66" s="7">
+        <v>207</v>
+      </c>
+      <c r="G66" s="7">
+        <v>1650</v>
+      </c>
+      <c r="H66" s="7">
+        <v>12.3</v>
+      </c>
+      <c r="I66" s="7">
+        <v>4141</v>
+      </c>
+      <c r="J66" s="7">
+        <v>3077</v>
+      </c>
+      <c r="K66" s="7">
+        <v>1064</v>
+      </c>
+      <c r="L66" s="7">
+        <v>606</v>
+      </c>
+      <c r="M66" s="7">
+        <v>355</v>
+      </c>
+      <c r="N66" s="7">
+        <v>152</v>
+      </c>
+      <c r="O66" s="7">
+        <v>99</v>
+      </c>
+      <c r="P66" s="7">
+        <v>38</v>
+      </c>
+      <c r="Q66" s="7">
+        <v>23.96</v>
+      </c>
+      <c r="R66" s="7">
+        <v>12.43</v>
+      </c>
+      <c r="S66" s="7">
+        <v>13.17</v>
+      </c>
+      <c r="T66" s="7">
+        <v>7.71</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20">
+      <c r="A67" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B67" s="7">
+        <v>8883</v>
+      </c>
+      <c r="C67" s="7">
+        <v>3258</v>
+      </c>
+      <c r="D67" s="7">
+        <v>1521</v>
+      </c>
+      <c r="E67" s="7">
+        <v>654</v>
+      </c>
+      <c r="F67" s="7">
+        <v>409</v>
+      </c>
+      <c r="G67" s="7">
+        <v>3041</v>
+      </c>
+      <c r="H67" s="7">
+        <v>9</v>
+      </c>
+      <c r="I67" s="7">
+        <v>11166</v>
+      </c>
+      <c r="J67" s="7">
+        <v>6659</v>
+      </c>
+      <c r="K67" s="7">
+        <v>4507</v>
+      </c>
+      <c r="L67" s="7">
+        <v>2388</v>
+      </c>
+      <c r="M67" s="7">
+        <v>2006</v>
+      </c>
+      <c r="N67" s="7">
+        <v>260</v>
+      </c>
+      <c r="O67" s="7">
+        <v>122</v>
+      </c>
+      <c r="P67" s="7">
+        <v>26.3</v>
+      </c>
+      <c r="Q67" s="7">
+        <v>29.09</v>
+      </c>
+      <c r="R67" s="7">
+        <v>17.12</v>
+      </c>
+      <c r="S67" s="7">
+        <v>26.88</v>
+      </c>
+      <c r="T67" s="7">
+        <v>22.58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20">
+      <c r="A68" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B68" s="7">
+        <v>1468</v>
+      </c>
+      <c r="C68" s="7">
+        <v>632</v>
+      </c>
+      <c r="D68" s="7">
+        <v>293</v>
+      </c>
+      <c r="E68" s="7">
+        <v>91</v>
+      </c>
+      <c r="F68" s="7">
+        <v>52</v>
+      </c>
+      <c r="G68" s="7">
+        <v>400</v>
+      </c>
+      <c r="H68" s="7">
+        <v>13.3</v>
+      </c>
+      <c r="I68" s="7">
+        <v>1867</v>
+      </c>
+      <c r="J68" s="7">
+        <v>1108</v>
+      </c>
+      <c r="K68" s="7">
+        <v>759</v>
+      </c>
+      <c r="L68" s="7">
+        <v>492</v>
+      </c>
+      <c r="M68" s="7">
+        <v>446</v>
+      </c>
+      <c r="N68" s="7">
+        <v>30</v>
+      </c>
+      <c r="O68" s="7">
+        <v>16</v>
+      </c>
+      <c r="P68" s="7">
+        <v>27.3</v>
+      </c>
+      <c r="Q68" s="7">
+        <v>29.7</v>
+      </c>
+      <c r="R68" s="7">
+        <v>19.96</v>
+      </c>
+      <c r="S68" s="7">
+        <v>33.51</v>
+      </c>
+      <c r="T68" s="7">
+        <v>30.38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20">
+      <c r="A69" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B69" s="7">
+        <v>1162</v>
+      </c>
+      <c r="C69" s="7">
+        <v>498</v>
+      </c>
+      <c r="D69" s="7">
+        <v>194</v>
+      </c>
+      <c r="E69" s="7">
+        <v>69</v>
+      </c>
+      <c r="F69" s="7">
+        <v>51</v>
+      </c>
+      <c r="G69" s="7">
+        <v>350</v>
+      </c>
+      <c r="H69" s="7">
+        <v>15</v>
+      </c>
+      <c r="I69" s="7">
+        <v>1459</v>
+      </c>
+      <c r="J69" s="7">
+        <v>769</v>
+      </c>
+      <c r="K69" s="7">
+        <v>690</v>
+      </c>
+      <c r="L69" s="7">
+        <v>344</v>
+      </c>
+      <c r="M69" s="7">
+        <v>301</v>
+      </c>
+      <c r="N69" s="7">
+        <v>25</v>
+      </c>
+      <c r="O69" s="7">
+        <v>18</v>
+      </c>
+      <c r="P69" s="7">
+        <v>19</v>
+      </c>
+      <c r="Q69" s="7">
+        <v>27.02</v>
+      </c>
+      <c r="R69" s="7">
+        <v>16.7</v>
+      </c>
+      <c r="S69" s="7">
+        <v>29.6</v>
+      </c>
+      <c r="T69" s="7">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20">
+      <c r="A70" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B70" s="7">
+        <v>284</v>
+      </c>
+      <c r="C70" s="7">
+        <v>142</v>
+      </c>
+      <c r="D70" s="7">
+        <v>35</v>
+      </c>
+      <c r="E70" s="7">
+        <v>18</v>
+      </c>
+      <c r="F70" s="7">
+        <v>9</v>
+      </c>
+      <c r="G70" s="7">
+        <v>80</v>
+      </c>
+      <c r="H70" s="7">
+        <v>10.7</v>
+      </c>
+      <c r="I70" s="7">
+        <v>293</v>
+      </c>
+      <c r="J70" s="7">
+        <v>147</v>
+      </c>
+      <c r="K70" s="7">
+        <v>146</v>
+      </c>
+      <c r="L70" s="7">
+        <v>72</v>
+      </c>
+      <c r="M70" s="7">
+        <v>62</v>
+      </c>
+      <c r="N70" s="7">
+        <v>7</v>
+      </c>
+      <c r="O70" s="7">
+        <v>3</v>
+      </c>
+      <c r="P70" s="7">
+        <v>28</v>
+      </c>
+      <c r="Q70" s="7">
+        <v>21.83</v>
+      </c>
+      <c r="R70" s="7">
+        <v>12.32</v>
+      </c>
+      <c r="S70" s="7">
+        <v>25.35</v>
+      </c>
+      <c r="T70" s="7">
+        <v>21.83</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20">
+      <c r="A71" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B71" s="7">
+        <v>9109</v>
+      </c>
+      <c r="C71" s="7">
+        <v>2785</v>
+      </c>
+      <c r="D71" s="7">
+        <v>1728</v>
+      </c>
+      <c r="E71" s="7">
+        <v>730</v>
+      </c>
+      <c r="F71" s="7">
+        <v>480</v>
+      </c>
+      <c r="G71" s="7">
+        <v>3386</v>
+      </c>
+      <c r="H71" s="7">
+        <v>7</v>
+      </c>
+      <c r="I71" s="7">
+        <v>12312</v>
+      </c>
+      <c r="J71" s="7">
+        <v>10775</v>
+      </c>
+      <c r="K71" s="7">
+        <v>1537</v>
+      </c>
+      <c r="L71" s="7">
+        <v>1627</v>
+      </c>
+      <c r="M71" s="7">
+        <v>1153</v>
+      </c>
+      <c r="N71" s="7">
+        <v>298</v>
+      </c>
+      <c r="O71" s="7">
+        <v>176</v>
+      </c>
+      <c r="P71" s="7">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="Q71" s="7">
+        <v>32.25</v>
+      </c>
+      <c r="R71" s="7">
+        <v>18.97</v>
+      </c>
+      <c r="S71" s="7">
+        <v>17.86</v>
+      </c>
+      <c r="T71" s="7">
+        <v>12.66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20">
+      <c r="A72" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B72" s="7">
+        <v>657</v>
+      </c>
+      <c r="C72" s="7">
+        <v>309</v>
+      </c>
+      <c r="D72" s="7">
+        <v>54</v>
+      </c>
+      <c r="E72" s="7">
+        <v>39</v>
+      </c>
+      <c r="F72" s="7">
+        <v>33</v>
+      </c>
+      <c r="G72" s="7">
+        <v>222</v>
+      </c>
+      <c r="H72" s="7">
+        <v>13.7</v>
+      </c>
+      <c r="I72" s="7">
+        <v>998</v>
+      </c>
+      <c r="J72" s="7">
+        <v>542</v>
+      </c>
+      <c r="K72" s="7">
+        <v>456</v>
+      </c>
+      <c r="L72" s="7">
+        <v>142</v>
+      </c>
+      <c r="M72" s="7">
+        <v>118</v>
+      </c>
+      <c r="N72" s="7">
+        <v>15</v>
+      </c>
+      <c r="O72" s="7">
+        <v>9</v>
+      </c>
+      <c r="P72" s="7">
+        <v>30.3</v>
+      </c>
+      <c r="Q72" s="7">
+        <v>19.18</v>
+      </c>
+      <c r="R72" s="7">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="S72" s="7">
+        <v>21.61</v>
+      </c>
+      <c r="T72" s="7">
+        <v>17.96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20">
+      <c r="A73" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B73" s="7">
+        <v>8553</v>
+      </c>
+      <c r="C73" s="7">
+        <v>3347</v>
+      </c>
+      <c r="D73" s="7">
+        <v>1281</v>
+      </c>
+      <c r="E73" s="7">
+        <v>669</v>
+      </c>
+      <c r="F73" s="7">
+        <v>378</v>
+      </c>
+      <c r="G73" s="7">
+        <v>2878</v>
+      </c>
+      <c r="H73" s="7">
+        <v>7</v>
+      </c>
+      <c r="I73" s="7">
+        <v>8550</v>
+      </c>
+      <c r="J73" s="7">
+        <v>6627</v>
+      </c>
+      <c r="K73" s="7">
+        <v>1923</v>
+      </c>
+      <c r="L73" s="7">
+        <v>1468</v>
+      </c>
+      <c r="M73" s="7">
+        <v>996</v>
+      </c>
+      <c r="N73" s="7">
+        <v>292</v>
+      </c>
+      <c r="O73" s="7">
+        <v>180</v>
+      </c>
+      <c r="P73" s="7">
+        <v>37</v>
+      </c>
+      <c r="Q73" s="7">
+        <v>27.22</v>
+      </c>
+      <c r="R73" s="7">
+        <v>14.98</v>
+      </c>
+      <c r="S73" s="7">
+        <v>17.16</v>
+      </c>
+      <c r="T73" s="7">
+        <v>11.65</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20">
+      <c r="A74" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B74" s="7">
+        <v>2506</v>
+      </c>
+      <c r="C74" s="7">
+        <v>1148</v>
+      </c>
+      <c r="D74" s="7">
+        <v>312</v>
+      </c>
+      <c r="E74" s="7">
+        <v>161</v>
+      </c>
+      <c r="F74" s="7">
+        <v>101</v>
+      </c>
+      <c r="G74" s="7">
+        <v>784</v>
+      </c>
+      <c r="H74" s="7">
+        <v>11.3</v>
+      </c>
+      <c r="I74" s="7">
+        <v>2282</v>
+      </c>
+      <c r="J74" s="7">
+        <v>1775</v>
+      </c>
+      <c r="K74" s="7">
+        <v>507</v>
+      </c>
+      <c r="L74" s="7">
+        <v>340</v>
+      </c>
+      <c r="M74" s="7">
+        <v>213</v>
+      </c>
+      <c r="N74" s="7">
+        <v>77</v>
+      </c>
+      <c r="O74" s="7">
+        <v>50</v>
+      </c>
+      <c r="P74" s="7">
+        <v>36</v>
+      </c>
+      <c r="Q74" s="7">
+        <v>22.91</v>
+      </c>
+      <c r="R74" s="7">
+        <v>12.45</v>
+      </c>
+      <c r="S74" s="7">
+        <v>13.57</v>
+      </c>
+      <c r="T74" s="7">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20">
+      <c r="A75" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B75" s="7">
+        <v>1520</v>
+      </c>
+      <c r="C75" s="7">
+        <v>606</v>
+      </c>
+      <c r="D75" s="7">
+        <v>358</v>
+      </c>
+      <c r="E75" s="7">
+        <v>73</v>
+      </c>
+      <c r="F75" s="7">
+        <v>59</v>
+      </c>
+      <c r="G75" s="7">
+        <v>424</v>
+      </c>
+      <c r="H75" s="7">
+        <v>12.7</v>
+      </c>
+      <c r="I75" s="7">
+        <v>1896</v>
+      </c>
+      <c r="J75" s="7">
+        <v>1136</v>
+      </c>
+      <c r="K75" s="7">
+        <v>760</v>
+      </c>
+      <c r="L75" s="7">
+        <v>659</v>
+      </c>
+      <c r="M75" s="7">
+        <v>609</v>
+      </c>
+      <c r="N75" s="7">
+        <v>35</v>
+      </c>
+      <c r="O75" s="7">
+        <v>15</v>
+      </c>
+      <c r="P75" s="7">
+        <v>22.7</v>
+      </c>
+      <c r="Q75" s="7">
+        <v>32.24</v>
+      </c>
+      <c r="R75" s="7">
+        <v>23.55</v>
+      </c>
+      <c r="S75" s="7">
+        <v>43.36</v>
+      </c>
+      <c r="T75" s="7">
+        <v>40.07</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:A16"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>